<commit_message>
save 25 07 2025
</commit_message>
<xml_diff>
--- a/4 четверть_5_JavaScript_Front_заготовки_scroll.xlsx
+++ b/4 четверть_5_JavaScript_Front_заготовки_scroll.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Machenike\Desktop\Homework_repo\GB_Developer_Workbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0F05E5-65D5-4748-9B13-E7BC4A5BB533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC603D5-D8EF-44D7-8C89-8D671385AAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Библиотеки" sheetId="25" r:id="rId1"/>
@@ -2426,12 +2426,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2725,8 +2733,8 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2739,39 +2747,42 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2782,107 +2793,104 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Гиперссылка 2" xfId="2" xr:uid="{A5746380-0C5B-42A9-896C-F81FD850516B}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{8BCFA195-9753-435C-B1BC-10F4F2F08605}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3264,42 +3272,42 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="22" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="71.1796875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" style="24" customWidth="1"/>
-    <col min="6" max="6" width="43.26953125" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="64.36328125" style="22" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="24" customWidth="1"/>
-    <col min="11" max="11" width="39.26953125" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="22" customWidth="1"/>
-    <col min="13" max="13" width="72.6328125" style="22" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="22" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="24" customWidth="1"/>
-    <col min="16" max="16" width="56.81640625" style="21" customWidth="1"/>
-    <col min="17" max="17" width="46.7265625" style="21" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="21" customWidth="1"/>
-    <col min="19" max="19" width="49.1796875" style="22" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" style="25"/>
-    <col min="21" max="21" width="67.7265625" style="21" customWidth="1"/>
-    <col min="22" max="22" width="68.36328125" style="22" customWidth="1"/>
-    <col min="23" max="24" width="59.36328125" style="22" customWidth="1"/>
-    <col min="25" max="25" width="59.6328125" style="22" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="22" customWidth="1"/>
-    <col min="27" max="27" width="41.26953125" style="22" customWidth="1"/>
-    <col min="28" max="16384" width="8.7265625" style="22"/>
+    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="24" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="22" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="22" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="24" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="22" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="22" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="22" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="24" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="22" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="25"/>
+    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="22" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="22" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="22" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="22" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="22" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="21"/>
       <c r="D1" s="21"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
@@ -3318,7 +3326,7 @@
       <c r="S2" s="27"/>
       <c r="U2" s="27"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>45</v>
       </c>
@@ -3332,7 +3340,7 @@
       <c r="U3" s="22"/>
       <c r="V3" s="21"/>
     </row>
-    <row r="4" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>48</v>
       </c>
@@ -3359,7 +3367,7 @@
       <c r="U4" s="21"/>
       <c r="V4" s="22"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>51</v>
       </c>
@@ -3370,7 +3378,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>54</v>
       </c>
@@ -3381,7 +3389,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>57</v>
       </c>
@@ -3395,7 +3403,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>61</v>
       </c>
@@ -3406,7 +3414,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>64</v>
       </c>
@@ -3417,7 +3425,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>67</v>
       </c>
@@ -3428,7 +3436,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>70</v>
       </c>
@@ -3465,38 +3473,38 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="71.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.81640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.7265625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.1796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" style="8"/>
-    <col min="21" max="21" width="67.7265625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.36328125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.36328125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.6328125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.26953125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="8"/>
+    <col min="21" max="21" width="67.77734375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -3515,7 +3523,7 @@
       <c r="S2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3524,12 +3532,12 @@
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -3543,18 +3551,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C7" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="145" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>8</v>
       </c>
@@ -3565,33 +3573,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C10" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="87" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C11" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:22" ht="174" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
       <c r="C14" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="145" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="144" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
@@ -3600,7 +3608,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -3617,38 +3625,38 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="71.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.81640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.7265625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.1796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" style="8"/>
-    <col min="21" max="21" width="67.7265625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.36328125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.36328125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.6328125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.26953125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="8"/>
+    <col min="21" max="21" width="67.77734375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -3667,7 +3675,7 @@
       <c r="S2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3676,12 +3684,12 @@
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="232" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="17" t="s">
         <v>31</v>
@@ -3690,33 +3698,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="290" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="288" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="C6" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="290" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="288" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="12"/>
       <c r="C7" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C11" s="13"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C13" s="12"/>
     </row>
   </sheetData>
@@ -3736,38 +3744,38 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="71.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.81640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.7265625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.1796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" style="8"/>
-    <col min="21" max="21" width="67.7265625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.36328125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.36328125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.6328125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.26953125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="8"/>
+    <col min="21" max="21" width="67.77734375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -3786,7 +3794,7 @@
       <c r="S2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3795,12 +3803,12 @@
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -3809,13 +3817,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>16</v>
       </c>
@@ -3826,7 +3834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -3835,16 +3843,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C11" s="13"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C13" s="12"/>
     </row>
   </sheetData>
@@ -3864,38 +3872,38 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="71.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.81640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.7265625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.1796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" style="8"/>
-    <col min="21" max="21" width="67.7265625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.36328125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.36328125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.6328125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.26953125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="8"/>
+    <col min="21" max="21" width="67.77734375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -3914,7 +3922,7 @@
       <c r="S2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3923,12 +3931,12 @@
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -3937,13 +3945,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="203" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="201.6" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="C6" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="203" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="12" t="s">
         <v>23</v>
@@ -3952,20 +3960,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C11" s="13"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C13" s="12"/>
     </row>
   </sheetData>
@@ -3985,38 +3993,38 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="71.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.81640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.7265625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.1796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" style="8"/>
-    <col min="21" max="21" width="67.7265625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.36328125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.36328125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.6328125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.26953125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="8"/>
+    <col min="21" max="21" width="67.77734375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -4035,7 +4043,7 @@
       <c r="S2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4044,7 +4052,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>38</v>
       </c>
@@ -4054,7 +4062,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>37</v>
       </c>
@@ -4062,72 +4070,72 @@
       <c r="C5" s="21"/>
       <c r="D5" s="22"/>
     </row>
-    <row r="6" spans="1:22" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="360" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="13"/>
     </row>
-    <row r="8" spans="1:22" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
       <c r="C8" s="30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="C9" s="31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="C10" s="31" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="C11" s="31" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="C12" s="31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="C13" s="31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="C14" s="31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="116" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="C15" s="31" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>75</v>
       </c>
       <c r="C16" s="19"/>
     </row>
-    <row r="17" spans="1:22" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="2"/>
       <c r="C17" s="31" t="s">
@@ -4150,7 +4158,7 @@
       <c r="U17" s="2"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -4171,7 +4179,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>74</v>
       </c>
@@ -4194,7 +4202,7 @@
       <c r="U19" s="2"/>
       <c r="V19" s="1"/>
     </row>
-    <row r="20" spans="1:22" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" s="7" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="31" t="s">
@@ -4217,23 +4225,23 @@
       <c r="U20" s="2"/>
       <c r="V20" s="1"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B24" s="21" t="s">
         <v>41</v>
       </c>
@@ -4257,42 +4265,42 @@
   </sheetPr>
   <dimension ref="A2:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="71.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.81640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.7265625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.1796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" style="8"/>
-    <col min="21" max="21" width="67.7265625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.36328125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.36328125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.6328125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.26953125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="8"/>
+    <col min="21" max="21" width="67.77734375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -4311,7 +4319,7 @@
       <c r="S2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>89</v>
       </c>
@@ -4323,7 +4331,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>88</v>
       </c>
@@ -4333,7 +4341,7 @@
       </c>
       <c r="D4" s="22"/>
     </row>
-    <row r="5" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>92</v>
       </c>
@@ -4343,7 +4351,7 @@
       <c r="C5" s="45"/>
       <c r="D5" s="46"/>
     </row>
-    <row r="6" spans="1:22" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>91</v>
       </c>
@@ -4351,18 +4359,18 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="31"/>
       <c r="C8" s="36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="38" t="s">
         <v>96</v>
       </c>
@@ -4372,7 +4380,7 @@
       <c r="C9" s="43"/>
       <c r="D9" s="44"/>
     </row>
-    <row r="10" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="31"/>
       <c r="B10" s="36" t="s">
         <v>98</v>
@@ -4381,7 +4389,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" s="2" t="s">
         <v>100</v>
@@ -4390,12 +4398,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A13" s="31"/>
       <c r="B13" s="36" t="s">
         <v>101</v>
@@ -4404,28 +4412,28 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
       <c r="B14" s="31"/>
       <c r="C14" s="36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="87" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="31"/>
       <c r="C15" s="36" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="31"/>
       <c r="C16" s="36" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="38" t="s">
         <v>106</v>
       </c>
@@ -4433,7 +4441,7 @@
       <c r="C17" s="38"/>
       <c r="D17" s="44"/>
     </row>
-    <row r="18" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="40" t="s">
         <v>123</v>
@@ -4442,19 +4450,19 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="31"/>
       <c r="C19" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="42" t="s">
         <v>115</v>
       </c>
       <c r="C20" s="36"/>
     </row>
-    <row r="21" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="36" t="s">
         <v>114</v>
       </c>
@@ -4463,14 +4471,14 @@
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="36" t="s">
@@ -4493,7 +4501,7 @@
       <c r="U23" s="2"/>
       <c r="V23" s="1"/>
     </row>
-    <row r="24" spans="1:22" s="7" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="31"/>
       <c r="B24" s="31"/>
       <c r="C24" s="39" t="s">
@@ -4516,7 +4524,7 @@
       <c r="U24" s="2"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37" t="s">
         <v>95</v>
       </c>
@@ -4539,7 +4547,7 @@
       <c r="U25" s="2"/>
       <c r="V25" s="1"/>
     </row>
-    <row r="26" spans="1:22" s="7" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="31"/>
       <c r="B26" s="31"/>
       <c r="C26" s="36" t="s">
@@ -4562,13 +4570,13 @@
       <c r="U26" s="2"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="42" t="s">
         <v>116</v>
       </c>
       <c r="B27" s="31"/>
     </row>
-    <row r="28" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="31"/>
       <c r="B28" s="36" t="s">
         <v>118</v>
@@ -4577,7 +4585,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="31"/>
       <c r="B29" s="36" t="s">
         <v>124</v>
@@ -4586,7 +4594,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="38" t="s">
         <v>125</v>
       </c>
@@ -4594,7 +4602,7 @@
       <c r="C30" s="45"/>
       <c r="D30" s="46"/>
     </row>
-    <row r="31" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="31"/>
       <c r="B31" s="40" t="s">
         <v>123</v>
@@ -4603,60 +4611,60 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="31"/>
       <c r="B32" s="31"/>
       <c r="C32" s="36" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="145" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:22" ht="144" x14ac:dyDescent="0.3">
       <c r="A33" s="31"/>
       <c r="B33" s="31"/>
       <c r="C33" s="36" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="145" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:22" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="31"/>
       <c r="B34" s="31"/>
       <c r="C34" s="36" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="37" t="s">
         <v>95</v>
       </c>
       <c r="B35" s="31"/>
       <c r="C35" s="36"/>
     </row>
-    <row r="36" spans="1:22" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A36" s="31"/>
       <c r="B36" s="31"/>
       <c r="C36" s="36" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="87" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" s="31"/>
       <c r="B37" s="31"/>
       <c r="C37" s="36" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="145" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" ht="144" x14ac:dyDescent="0.3">
       <c r="A38" s="31"/>
       <c r="B38" s="31"/>
       <c r="C38" s="36" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="31"/>
       <c r="B39" s="31"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
@@ -4675,7 +4683,7 @@
       <c r="S41" s="5"/>
       <c r="U41" s="5"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="22"/>
       <c r="B42" s="21"/>
       <c r="C42" s="34" t="s">
@@ -4685,12 +4693,12 @@
       <c r="U42" s="1"/>
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="51" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:22" ht="331.2" x14ac:dyDescent="0.3">
       <c r="C44" s="50" t="s">
         <v>140</v>
       </c>
@@ -4713,38 +4721,38 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="71.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.81640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.7265625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.1796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" style="8"/>
-    <col min="21" max="21" width="67.7265625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.36328125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.36328125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.6328125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.26953125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="8"/>
+    <col min="21" max="21" width="67.77734375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -4763,7 +4771,7 @@
       <c r="S2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="49" t="s">
         <v>139</v>
       </c>
@@ -4771,7 +4779,7 @@
       <c r="C3" s="21"/>
       <c r="D3" s="22"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>37</v>
       </c>
@@ -4779,31 +4787,31 @@
       <c r="C4" s="21"/>
       <c r="D4" s="22"/>
     </row>
-    <row r="5" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="216" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>75</v>
       </c>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:22" s="7" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="2"/>
       <c r="C9" s="47" t="s">
@@ -4826,7 +4834,7 @@
       <c r="U9" s="2"/>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:22" s="7" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" s="7" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="48" t="s">
@@ -4849,7 +4857,7 @@
       <c r="U10" s="2"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>87</v>
       </c>
@@ -4872,7 +4880,7 @@
       <c r="U11" s="2"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:22" s="7" customFormat="1" ht="290" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" s="7" customFormat="1" ht="288" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="47" t="s">
@@ -4895,7 +4903,7 @@
       <c r="U12" s="2"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="22"/>

</xml_diff>